<commit_message>
Add *.py version + write function increase rate
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s\YandexDisk\Сергей\СРВН\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergey.reznikov\JupiterProjects\s-alerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBA6256-0326-4ED9-A617-140EB9C0EE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B484583-7D61-403D-BAA1-FBF3769F876F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4176" yWindow="1536" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{165519FD-E877-4780-B637-793905203CD6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{165519FD-E877-4780-B637-793905203CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -105,7 +96,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -121,9 +112,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,7 +152,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -267,7 +258,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -498,7 +489,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +616,7 @@
         <v>28</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>